<commit_message>
[FIX] Fix socket.io and Fix template and validation of CSV in User Account
</commit_message>
<xml_diff>
--- a/client/public/UserAccountTemplate.xlsx
+++ b/client/public/UserAccountTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IPIS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IPIS\Downloads\updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E16107-FA5C-435A-8513-D89B3E7F9063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC0312C-9237-4554-9103-022DA4BB1B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FF03A47-A5E5-4841-B4E1-B0CC0FE712F1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>User Type</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
     <t>Guidance Counselor</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Bachelor of Science in Public Administration (BSPA)</t>
   </si>
   <si>
-    <t>Raphael Bartolome</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -136,13 +130,53 @@
   </si>
   <si>
     <t>Year Section</t>
+  </si>
+  <si>
+    <t>College of Education</t>
+  </si>
+  <si>
+    <t>College of Engineering and Information Technology</t>
+  </si>
+  <si>
+    <t>College of Arts and Sciences</t>
+  </si>
+  <si>
+    <t>College of Business Administration, Public Administration and Accountancy</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Department </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(FOR STUDENTS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Colleges </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(FOR GUIDANCE Counselors)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +210,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -246,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -260,12 +300,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -575,28 +623,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59157DB-6347-4D6E-BBEA-561488E8F987}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="43.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="40" style="1" customWidth="1"/>
+    <col min="11" max="11" width="45.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -604,66 +653,71 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{91F76DDD-DDE1-4FEE-BC0B-1E97FD6B2EBC}">
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>INDIRECT("A" &amp; ROW())="student"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="5">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Password must 8 characters or more!" sqref="D2:D1048576" xr:uid="{91F76DDD-DDE1-4FEE-BC0B-1E97FD6B2EBC}">
       <formula1>8</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{D4AF8EB8-C850-4D80-9F66-8631D85A12FD}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Use the PLV domain (e.g. name@plv.edu.ph)" sqref="C2:C1048576" xr:uid="{D4AF8EB8-C850-4D80-9F66-8631D85A12FD}">
       <formula1>ISNUMBER(MATCH("*@plv.edu.ph",C2,0))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{2A51EBE6-C5A4-46E2-8EFC-7DF9501CDC98}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Contact number must follow the 11-number format!" sqref="G2:G1048576" xr:uid="{2A51EBE6-C5A4-46E2-8EFC-7DF9501CDC98}">
       <formula1>11</formula1>
       <formula2>11</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{08EE51FE-A53F-46A8-8AFF-18620A4FD6D6}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Birthday must follow the mm/dd/yyyy format!" sqref="H2:H1048576" xr:uid="{08EE51FE-A53F-46A8-8AFF-18620A4FD6D6}">
       <formula1>21916</formula1>
       <formula2>38322</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="The Guidance Counselor does not have any year and section details!" sqref="I2:I1048576" xr:uid="{EECB96DA-6BF1-4C00-BB4E-4E19B515EC8C}">
+      <formula1>INDIRECT("A" &amp; ROW())="student"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E8D04D7-E74F-49D0-9858-38FBE1F1B077}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
@@ -682,6 +736,12 @@
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5650544-F140-48D5-A029-34B8B155D9D2}">
+          <x14:formula1>
+            <xm:f>Sheet2!$D$1:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -693,52 +753,59 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="133.85546875" customWidth="1"/>
+    <col min="4" max="4" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
@@ -746,9 +813,11 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
@@ -756,7 +825,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -766,7 +835,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -776,7 +845,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -786,7 +855,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -796,7 +865,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -806,7 +875,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -816,7 +885,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -826,7 +895,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -836,7 +905,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -846,7 +915,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -856,7 +925,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -866,7 +935,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -876,7 +945,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>

</xml_diff>